<commit_message>
added validate met method and added xpath for testdata updated
</commit_message>
<xml_diff>
--- a/src/main/resources/nameaddress.xlsx
+++ b/src/main/resources/nameaddress.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHISH\Downloads\Testing baba\testing baba 0530\javaworkspace\tesngAut\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHISH\IdeaProjects\TestingBABAmvn\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7AAC6D-778E-49DC-9B0E-5E2CE7924AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA649E58-E621-44DC-AB39-C70A5EF206EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -191,6 +192,24 @@
   </si>
   <si>
     <t>Nitishdd</t>
+  </si>
+  <si>
+    <t>Nitish</t>
+  </si>
+  <si>
+    <t>Ghansh</t>
+  </si>
+  <si>
+    <t>mohit</t>
+  </si>
+  <si>
+    <t>ghanesh@gmail.com</t>
+  </si>
+  <si>
+    <t>mohdit@gmail.com</t>
+  </si>
+  <si>
+    <t>nitish@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -464,8 +483,8 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="A7:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -754,4 +773,209 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3353307-8A55-4757-8319-62F21DE0CADA}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{5DAC7A13-636A-4D39-AA0E-2223C85C136A}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{45B84B36-3D65-4ADB-B48C-0A14793C5151}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{CFD8E16B-6BBD-47F5-BDA3-E8E9EC450654}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>